<commit_message>
new gerber files. Complete BOM.
</commit_message>
<xml_diff>
--- a/main board BOM.xlsx
+++ b/main board BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Description</t>
   </si>
@@ -33,51 +33,24 @@
     <t>1k surface mount resistors 0805</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/8145889/</t>
-  </si>
-  <si>
-    <t>10uF surface mount capacitors 0805</t>
-  </si>
-  <si>
-    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/8467293/</t>
-  </si>
-  <si>
     <t>10 pin female header</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/pcb-headers/2204894/</t>
-  </si>
-  <si>
-    <t>2 pin header</t>
-  </si>
-  <si>
     <t>http://china.rs-online.com//web/p/pcb-headers/2518086/</t>
   </si>
   <si>
     <t>220uF capacitors</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/aluminium-capacitors/5261480/</t>
-  </si>
-  <si>
     <t>500k surface mount resistors 0805</t>
   </si>
   <si>
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791437/</t>
   </si>
   <si>
-    <t>220k surface mount resistors 0805</t>
-  </si>
-  <si>
-    <t>http://china.rs-online.com//web/p/surface-mount-fixed-resistors/2232574/</t>
-  </si>
-  <si>
     <t>2A 100ohm ferrite bead</t>
   </si>
   <si>
-    <t>http://china.rs-online.com//web/p/ferrite-beads/7926246/</t>
-  </si>
-  <si>
     <t>L7809CV voltage regulator IC (TO-220V)</t>
   </si>
   <si>
@@ -118,6 +91,117 @@
   </si>
   <si>
     <t>http://china.rs-online.com/web/p/linear-voltage-regulators/5166240/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230427/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/ferrite-beads/6694159/?searchTerm=742792312&amp;relevancy-data=636F3D3126696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E285C642B5B2D5C2E5C732F5D292B285C642B293F247C5E5C642B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F4F525F4D554C54495F4E554D455249432677633D424F5448267573743D373432373932333132267374613D37343237393233313226</t>
+  </si>
+  <si>
+    <t>Label on PCB</t>
+  </si>
+  <si>
+    <t>U21</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U33</t>
+  </si>
+  <si>
+    <t>U32</t>
+  </si>
+  <si>
+    <t>U15</t>
+  </si>
+  <si>
+    <t>4k7 surface mounts resistor 0805</t>
+  </si>
+  <si>
+    <t>R2, R3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/aluminium-capacitors/3150726/</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>20 Ohm surface mount resistor 0805</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>1uF SMT capacitors</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/4515770/</t>
+  </si>
+  <si>
+    <t>C1, C3, C4, C17</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/2644416/</t>
+  </si>
+  <si>
+    <t>100nF SMT capacitors</t>
+  </si>
+  <si>
+    <t>C2,C8</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/7217615/</t>
+  </si>
+  <si>
+    <t>10uF capacitor</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/aluminium-capacitors/0117035/</t>
+  </si>
+  <si>
+    <t>U4, C5, U8</t>
+  </si>
+  <si>
+    <t>C16, C23</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230528/</t>
+  </si>
+  <si>
+    <t>2 pin male header</t>
+  </si>
+  <si>
+    <t>J6, J7,J3</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>U3, U34</t>
+  </si>
+  <si>
+    <t>3 pin male header</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/pcb-headers/2518092/</t>
+  </si>
+  <si>
+    <t>J2, J4</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/pcb-sockets/7655745/</t>
+  </si>
+  <si>
+    <t>J1, J5, Header for Arduino</t>
   </si>
 </sst>
 </file>
@@ -147,12 +231,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -168,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -179,6 +269,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -494,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C17"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,203 +599,304 @@
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
+      <c r="D21" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4" display="http://china.rs-online.com/web/p/pcb-headers/2518086/"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7" display="http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2232574/"/>
-    <hyperlink ref="B10" r:id="rId8" display="http://china.rs-online.com/web/p/ferrite-beads/7926246/"/>
-    <hyperlink ref="B11" r:id="rId9" display="http://china.rs-online.com/web/p/linear-voltage-regulators/7140666/"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B15" r:id="rId13" display="http://china.rs-online.com/web/p/tvs-diodes/6287691/"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B8" r:id="rId1" display="http://china.rs-online.com/web/p/pcb-headers/2518086/"/>
+    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B12" r:id="rId3" display="http://china.rs-online.com/web/p/linear-voltage-regulators/7140666/"/>
+    <hyperlink ref="B13" r:id="rId4"/>
+    <hyperlink ref="B14" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
+    <hyperlink ref="B16" r:id="rId7" display="http://china.rs-online.com/web/p/tvs-diodes/6287691/"/>
+    <hyperlink ref="B17" r:id="rId8"/>
+    <hyperlink ref="B18" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="B4" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>